<commit_message>
added image testing to rspec tests
</commit_message>
<xml_diff>
--- a/director/dataload_files/event_types_load.xlsx
+++ b/director/dataload_files/event_types_load.xlsx
@@ -24,75 +24,36 @@
     <t>Food</t>
   </si>
   <si>
-    <t>event_types/FOOD.FancyPants.MoodyKurtArmstrong.jpg</t>
-  </si>
-  <si>
     <t>Fancy Pants Dinner</t>
   </si>
   <si>
-    <t>event_types/FOOD.FancyPants.Brickhouse_Ban.jpg</t>
-  </si>
-  <si>
     <t>Good Eats</t>
   </si>
   <si>
-    <t>event_types/FOOD.GoodEats2.jpg</t>
-  </si>
-  <si>
     <t>Grab-and-Go</t>
   </si>
   <si>
-    <t>event_types/FOOD.GrabandGo.Night.Kurt Armstrong.jpg</t>
-  </si>
-  <si>
     <t>Drinks</t>
   </si>
   <si>
-    <t>event_types/DRINKS.Beers.JPG</t>
-  </si>
-  <si>
     <t>Top Shelf Cocktails</t>
   </si>
   <si>
-    <t>event_types/DRINKS.TopShelf.Martini.Kurt Armstrong.jpg</t>
-  </si>
-  <si>
     <t>Hot Spot</t>
   </si>
   <si>
-    <t>event_types/DRINKS.HotSpot.KurtArmstrong.jpg</t>
-  </si>
-  <si>
     <t>Casual, But Nice Drinks</t>
   </si>
   <si>
-    <t>event_types/DRINKS.Casual.KurtArmstrong.jpg</t>
-  </si>
-  <si>
     <t>Brew Pub</t>
   </si>
   <si>
-    <t>event_types/DRINKS.BrewPub.Kurt Armstrong.jpg</t>
-  </si>
-  <si>
     <t>Dive Bar</t>
   </si>
   <si>
-    <t>event_types/DRINKS.DiveBar.jpg</t>
-  </si>
-  <si>
-    <t>event_types/OUTSIDE.GetPhysical.MtnBikeclimb.jpg</t>
-  </si>
-  <si>
     <t>Get Physical</t>
   </si>
   <si>
-    <t>event_types/OUTSIDE.GetPhysical.Hike.jpg</t>
-  </si>
-  <si>
-    <t>event_types/FOOD.Grub.JPG</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -168,40 +129,79 @@
     <t>Art Show</t>
   </si>
   <si>
-    <t>event_types/OUTSIDE.GetPhysical.RockClimb.jpg</t>
-  </si>
-  <si>
-    <t>event_types/MUSIC.Headliners.Concerts_Ben Harper.jpg</t>
-  </si>
-  <si>
-    <t>event_types/MUSIC.OutdoorConcert.LesSchwab.JPG</t>
-  </si>
-  <si>
-    <t>event_types/MUSIC.Mellow.Concert_Franchot Tone_Ben Moon.jpg</t>
-  </si>
-  <si>
-    <t>event_types/MUSIC.Up&amp;Coming.indoor.MoWo.jpg</t>
-  </si>
-  <si>
-    <t>event_types/CULTURE.Classic.Ballet.jpg</t>
-  </si>
-  <si>
-    <t>event_types/CULTURE.Classic.DressedUp.jpg</t>
-  </si>
-  <si>
-    <t>event_types/CULTURE.Underground.jpg</t>
-  </si>
-  <si>
-    <t>event_types/CULTURE.ArtShow.jpg</t>
-  </si>
-  <si>
     <t>event_type_name</t>
   </si>
   <si>
-    <t>event_types/MOVIE.Fantasy.jpg</t>
-  </si>
-  <si>
     <t>need</t>
+  </si>
+  <si>
+    <t>FOOD.FancyPants.MoodyKurtArmstrong.jpg</t>
+  </si>
+  <si>
+    <t>DRINKS.Beers.JPG</t>
+  </si>
+  <si>
+    <t>DRINKS.TopShelf.Martini.Kurt Armstrong.jpg</t>
+  </si>
+  <si>
+    <t>FOOD.FancyPants.Brickhouse_Ban.jpg</t>
+  </si>
+  <si>
+    <t>FOOD.GoodEats2.jpg</t>
+  </si>
+  <si>
+    <t>FOOD.GrabandGo.Night.Kurt Armstrong.jpg</t>
+  </si>
+  <si>
+    <t>FOOD.Grub.JPG</t>
+  </si>
+  <si>
+    <t>DRINKS.HotSpot.KurtArmstrong.jpg</t>
+  </si>
+  <si>
+    <t>DRINKS.Casual.KurtArmstrong.jpg</t>
+  </si>
+  <si>
+    <t>DRINKS.BrewPub.Kurt Armstrong.jpg</t>
+  </si>
+  <si>
+    <t>DRINKS.DiveBar.jpg</t>
+  </si>
+  <si>
+    <t>OUTSIDE.GetPhysical.MtnBikeclimb.jpg</t>
+  </si>
+  <si>
+    <t>OUTSIDE.GetPhysical.Hike.jpg</t>
+  </si>
+  <si>
+    <t>OUTSIDE.GetPhysical.RockClimb.jpg</t>
+  </si>
+  <si>
+    <t>MUSIC.Headliners.Concerts_Ben Harper.jpg</t>
+  </si>
+  <si>
+    <t>MUSIC.OutdoorConcert.LesSchwab.JPG</t>
+  </si>
+  <si>
+    <t>MUSIC.Mellow.Concert_Franchot Tone_Ben Moon.jpg</t>
+  </si>
+  <si>
+    <t>MUSIC.Up&amp;Coming.indoor.MoWo.jpg</t>
+  </si>
+  <si>
+    <t>MOVIE.Fantasy.jpg</t>
+  </si>
+  <si>
+    <t>CULTURE.Classic.DressedUp.jpg</t>
+  </si>
+  <si>
+    <t>CULTURE.Classic.Ballet.jpg</t>
+  </si>
+  <si>
+    <t>CULTURE.Underground.jpg</t>
+  </si>
+  <si>
+    <t>CULTURE.ArtShow.jpg</t>
   </si>
 </sst>
 </file>
@@ -270,10 +270,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="46">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -329,7 +333,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="46">
+  <cellStyles count="50">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -354,6 +358,8 @@
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
@@ -375,6 +381,8 @@
     <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -708,7 +716,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -722,19 +730,19 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -743,7 +751,7 @@
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -751,13 +759,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -765,13 +773,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -779,13 +787,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -793,13 +801,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -807,11 +815,11 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -819,13 +827,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1">
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -833,13 +841,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1">
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -847,13 +855,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1">
         <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -861,13 +869,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1">
         <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -875,13 +883,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1">
         <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -889,11 +897,11 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -901,13 +909,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C14" s="1">
         <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -915,13 +923,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C15" s="2">
         <v>12</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -929,13 +937,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C16" s="2">
         <v>12</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -943,10 +951,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="24">
@@ -954,13 +962,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C18" s="2">
         <v>17</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -968,13 +976,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C19" s="2">
         <v>17</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -982,13 +990,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C20" s="2">
         <v>17</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -996,13 +1004,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C21" s="2">
         <v>17</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1010,13 +1018,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C22" s="2">
         <v>17</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1024,10 +1032,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1035,13 +1043,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C24" s="2">
         <v>23</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1049,13 +1057,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C25" s="2">
         <v>23</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1063,13 +1071,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C26" s="2">
         <v>23</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1077,13 +1085,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C27" s="2">
         <v>23</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1091,13 +1099,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C28" s="2">
         <v>23</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1105,13 +1113,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C29" s="2">
         <v>23</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1119,10 +1127,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1130,13 +1138,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C31" s="2">
         <v>30</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1144,13 +1152,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C32" s="2">
         <v>30</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1158,13 +1166,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C33" s="2">
         <v>30</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1172,13 +1180,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C34" s="2">
         <v>30</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>